<commit_message>
Updated IT_Stocks.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/IT_Stocks.xlsx
+++ b/NAV/IT_Stocks.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J596"/>
+  <dimension ref="A1:J612"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
       <selection activeCell="D602" sqref="D602"/>
@@ -18944,13 +18944,564 @@
       </c>
     </row>
     <row r="595">
-      <c r="A595" s="6" t="n"/>
+      <c r="A595" s="6" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
       <c r="B595" s="6" t="n"/>
-      <c r="H595" s="6" t="n"/>
-      <c r="J595" s="6" t="n"/>
+      <c r="C595" t="n">
+        <v>1933.349975585938</v>
+      </c>
+      <c r="D595" t="n">
+        <v>1751.849975585938</v>
+      </c>
+      <c r="E595" t="n">
+        <v>1061.300048828125</v>
+      </c>
+      <c r="F595" t="n">
+        <v>1857.849975585938</v>
+      </c>
+      <c r="G595" t="n">
+        <v>1726.550048828125</v>
+      </c>
+      <c r="H595" s="6" t="n">
+        <v>37876.40014648438</v>
+      </c>
+      <c r="I595" t="n">
+        <v>0.00363547585698216</v>
+      </c>
+      <c r="J595" s="6" t="n">
+        <v>178.9686390577944</v>
+      </c>
     </row>
     <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
       <c r="B596" s="6" t="n"/>
+      <c r="C596" t="n">
+        <v>1943.699951171875</v>
+      </c>
+      <c r="D596" t="n">
+        <v>1753.25</v>
+      </c>
+      <c r="E596" t="n">
+        <v>1065.599975585938</v>
+      </c>
+      <c r="F596" t="n">
+        <v>1815.150024414062</v>
+      </c>
+      <c r="G596" t="n">
+        <v>1772.25</v>
+      </c>
+      <c r="H596" t="n">
+        <v>37943.19958496094</v>
+      </c>
+      <c r="I596" t="n">
+        <v>0.001763616347335551</v>
+      </c>
+      <c r="J596" t="n">
+        <v>179.2842710752971</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C597" t="n">
+        <v>1964.5</v>
+      </c>
+      <c r="D597" t="n">
+        <v>1806.650024414062</v>
+      </c>
+      <c r="E597" t="n">
+        <v>1050.949951171875</v>
+      </c>
+      <c r="F597" t="n">
+        <v>1766.300048828125</v>
+      </c>
+      <c r="G597" t="n">
+        <v>1749.5</v>
+      </c>
+      <c r="H597" t="n">
+        <v>38025.74987792969</v>
+      </c>
+      <c r="I597" t="n">
+        <v>0.002175628146063607</v>
+      </c>
+      <c r="J597" t="n">
+        <v>179.674326981595</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C598" t="n">
+        <v>1941.25</v>
+      </c>
+      <c r="D598" t="n">
+        <v>1790.449951171875</v>
+      </c>
+      <c r="E598" t="n">
+        <v>1068.800048828125</v>
+      </c>
+      <c r="F598" t="n">
+        <v>1769.300048828125</v>
+      </c>
+      <c r="G598" t="n">
+        <v>1718.75</v>
+      </c>
+      <c r="H598" t="n">
+        <v>37895.55029296875</v>
+      </c>
+      <c r="I598" t="n">
+        <v>-0.003423984678248408</v>
+      </c>
+      <c r="J598" t="n">
+        <v>179.0591248389355</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C599" t="n">
+        <v>1922.449951171875</v>
+      </c>
+      <c r="D599" t="n">
+        <v>1785.25</v>
+      </c>
+      <c r="E599" t="n">
+        <v>1056.199951171875</v>
+      </c>
+      <c r="F599" t="n">
+        <v>1749.699951171875</v>
+      </c>
+      <c r="G599" t="n">
+        <v>1729.550048828125</v>
+      </c>
+      <c r="H599" t="n">
+        <v>37618.74926757812</v>
+      </c>
+      <c r="I599" t="n">
+        <v>-0.007304314708473397</v>
+      </c>
+      <c r="J599" t="n">
+        <v>177.7512206396881</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>1933.150024414062</v>
+      </c>
+      <c r="D600" t="n">
+        <v>1790.550048828125</v>
+      </c>
+      <c r="E600" t="n">
+        <v>1074.900024414062</v>
+      </c>
+      <c r="F600" t="n">
+        <v>1722.900024414062</v>
+      </c>
+      <c r="G600" t="n">
+        <v>1720.75</v>
+      </c>
+      <c r="H600" t="n">
+        <v>37761.05065917969</v>
+      </c>
+      <c r="I600" t="n">
+        <v>0.003782725220059497</v>
+      </c>
+      <c r="J600" t="n">
+        <v>178.4236046648982</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>1901.849975585938</v>
+      </c>
+      <c r="D601" t="n">
+        <v>1756.099975585938</v>
+      </c>
+      <c r="E601" t="n">
+        <v>1112.650024414062</v>
+      </c>
+      <c r="F601" t="n">
+        <v>1730.300048828125</v>
+      </c>
+      <c r="G601" t="n">
+        <v>1715</v>
+      </c>
+      <c r="H601" t="n">
+        <v>37713.70007324219</v>
+      </c>
+      <c r="I601" t="n">
+        <v>-0.001253953084220899</v>
+      </c>
+      <c r="J601" t="n">
+        <v>178.1998698355308</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C602" t="n">
+        <v>1894.650024414062</v>
+      </c>
+      <c r="D602" t="n">
+        <v>1746.75</v>
+      </c>
+      <c r="E602" t="n">
+        <v>1077.550048828125</v>
+      </c>
+      <c r="F602" t="n">
+        <v>1750.400024414062</v>
+      </c>
+      <c r="G602" t="n">
+        <v>1741.199951171875</v>
+      </c>
+      <c r="H602" t="n">
+        <v>37455.65051269531</v>
+      </c>
+      <c r="I602" t="n">
+        <v>-0.006842329446480399</v>
+      </c>
+      <c r="J602" t="n">
+        <v>176.9805676187962</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C603" t="n">
+        <v>1912.300048828125</v>
+      </c>
+      <c r="D603" t="n">
+        <v>1779.099975585938</v>
+      </c>
+      <c r="E603" t="n">
+        <v>1091</v>
+      </c>
+      <c r="F603" t="n">
+        <v>1756.349975585938</v>
+      </c>
+      <c r="G603" t="n">
+        <v>1745.150024414062</v>
+      </c>
+      <c r="H603" t="n">
+        <v>37856.65014648438</v>
+      </c>
+      <c r="I603" t="n">
+        <v>0.01070598503296977</v>
+      </c>
+      <c r="J603" t="n">
+        <v>178.8753189268495</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C604" t="n">
+        <v>1910.150024414062</v>
+      </c>
+      <c r="D604" t="n">
+        <v>1778.75</v>
+      </c>
+      <c r="E604" t="n">
+        <v>1077.849975585938</v>
+      </c>
+      <c r="F604" t="n">
+        <v>1789.349975585938</v>
+      </c>
+      <c r="G604" t="n">
+        <v>1782.650024414062</v>
+      </c>
+      <c r="H604" t="n">
+        <v>37910.79992675781</v>
+      </c>
+      <c r="I604" t="n">
+        <v>0.001430390170918655</v>
+      </c>
+      <c r="J604" t="n">
+        <v>179.1311804248624</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>1950.449951171875</v>
+      </c>
+      <c r="D605" t="n">
+        <v>1807.599975585938</v>
+      </c>
+      <c r="E605" t="n">
+        <v>1083.75</v>
+      </c>
+      <c r="F605" t="n">
+        <v>1838.050048828125</v>
+      </c>
+      <c r="G605" t="n">
+        <v>1812.75</v>
+      </c>
+      <c r="H605" t="n">
+        <v>38550.34973144531</v>
+      </c>
+      <c r="I605" t="n">
+        <v>0.01686985782212682</v>
+      </c>
+      <c r="J605" t="n">
+        <v>182.1530979701396</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>1944.099975585938</v>
+      </c>
+      <c r="D606" t="n">
+        <v>1812.800048828125</v>
+      </c>
+      <c r="E606" t="n">
+        <v>1089.699951171875</v>
+      </c>
+      <c r="F606" t="n">
+        <v>1826.050048828125</v>
+      </c>
+      <c r="G606" t="n">
+        <v>1814.099975585938</v>
+      </c>
+      <c r="H606" t="n">
+        <v>38552.5498046875</v>
+      </c>
+      <c r="I606" t="n">
+        <v>5.707012407186833e-05</v>
+      </c>
+      <c r="J606" t="n">
+        <v>182.1634934700408</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>1950.25</v>
+      </c>
+      <c r="D607" t="n">
+        <v>1811.849975585938</v>
+      </c>
+      <c r="E607" t="n">
+        <v>1094.650024414062</v>
+      </c>
+      <c r="F607" t="n">
+        <v>1757.849975585938</v>
+      </c>
+      <c r="G607" t="n">
+        <v>1797.199951171875</v>
+      </c>
+      <c r="H607" t="n">
+        <v>38385.89990234375</v>
+      </c>
+      <c r="I607" t="n">
+        <v>-0.004322668751821118</v>
+      </c>
+      <c r="J607" t="n">
+        <v>181.3760610290953</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>1952.550048828125</v>
+      </c>
+      <c r="D608" t="n">
+        <v>1813.75</v>
+      </c>
+      <c r="E608" t="n">
+        <v>1080.300048828125</v>
+      </c>
+      <c r="F608" t="n">
+        <v>1741.150024414062</v>
+      </c>
+      <c r="G608" t="n">
+        <v>1848.5</v>
+      </c>
+      <c r="H608" t="n">
+        <v>38346.90075683594</v>
+      </c>
+      <c r="I608" t="n">
+        <v>-0.001015975803798501</v>
+      </c>
+      <c r="J608" t="n">
+        <v>181.1917873397015</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C609" t="n">
+        <v>1892.150024414062</v>
+      </c>
+      <c r="D609" t="n">
+        <v>1756.5</v>
+      </c>
+      <c r="E609" t="n">
+        <v>1065.800048828125</v>
+      </c>
+      <c r="F609" t="n">
+        <v>1727.25</v>
+      </c>
+      <c r="G609" t="n">
+        <v>1805.599975585938</v>
+      </c>
+      <c r="H609" t="n">
+        <v>37454.75048828125</v>
+      </c>
+      <c r="I609" t="n">
+        <v>-0.023265250931541</v>
+      </c>
+      <c r="J609" t="n">
+        <v>176.9763149405089</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C610" t="n">
+        <v>1894.199951171875</v>
+      </c>
+      <c r="D610" t="n">
+        <v>1736.5</v>
+      </c>
+      <c r="E610" t="n">
+        <v>1060.75</v>
+      </c>
+      <c r="F610" t="n">
+        <v>1676.449951171875</v>
+      </c>
+      <c r="G610" t="n">
+        <v>1877.449951171875</v>
+      </c>
+      <c r="H610" t="n">
+        <v>37317.94946289062</v>
+      </c>
+      <c r="I610" t="n">
+        <v>-0.003652434567236724</v>
+      </c>
+      <c r="J610" t="n">
+        <v>176.329920530238</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>1905.75</v>
+      </c>
+      <c r="D611" t="n">
+        <v>1760.050048828125</v>
+      </c>
+      <c r="E611" t="n">
+        <v>1114.699951171875</v>
+      </c>
+      <c r="F611" t="n">
+        <v>1662</v>
+      </c>
+      <c r="G611" t="n">
+        <v>1931.449951171875</v>
+      </c>
+      <c r="H611" t="n">
+        <v>38001.24975585938</v>
+      </c>
+      <c r="I611" t="n">
+        <v>0.01831023147850691</v>
+      </c>
+      <c r="J611" t="n">
+        <v>179.5585621917334</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>1896.449951171875</v>
+      </c>
+      <c r="D612" t="n">
+        <v>1752.800048828125</v>
+      </c>
+      <c r="E612" t="n">
+        <v>1106.699951171875</v>
+      </c>
+      <c r="F612" t="n">
+        <v>1692.900024414062</v>
+      </c>
+      <c r="G612" t="n">
+        <v>1920.400024414062</v>
+      </c>
+      <c r="H612" t="n">
+        <v>37915.79968261719</v>
+      </c>
+      <c r="I612" t="n">
+        <v>-0.002248612184892999</v>
+      </c>
+      <c r="J612" t="n">
+        <v>179.1548046208872</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>